<commit_message>
updated activity tracker with work done 12/13 for phase 5
</commit_message>
<xml_diff>
--- a/ActivityTrackerPhase5.xlsx
+++ b/ActivityTrackerPhase5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jocel\PycharmProjects\Programming_Project\NetworkDesign_ProgrammingProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael Burton\Documents\GitHub\NetworkDesign_ProgrammingProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FB9C448-1933-41B3-A8CA-5BC92DBAD07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5458EFCF-6401-4022-A972-360F9AC40809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tracker" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="17">
   <si>
     <t>Project</t>
   </si>
@@ -794,22 +794,22 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomLeft" activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.59765625" customWidth="1"/>
-    <col min="2" max="3" width="22.59765625" customWidth="1"/>
-    <col min="4" max="5" width="15.59765625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="2.8984375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.59765625" customWidth="1"/>
-    <col min="8" max="8" width="2.8984375" customWidth="1"/>
-    <col min="9" max="9" width="25.59765625" customWidth="1"/>
-    <col min="10" max="10" width="19.09765625" customWidth="1"/>
+    <col min="1" max="1" width="2.58203125" customWidth="1"/>
+    <col min="2" max="3" width="22.58203125" customWidth="1"/>
+    <col min="4" max="5" width="15.58203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="2.9140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.58203125" customWidth="1"/>
+    <col min="8" max="8" width="2.9140625" customWidth="1"/>
+    <col min="9" max="9" width="25.58203125" customWidth="1"/>
+    <col min="10" max="10" width="19.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:10" ht="65.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>8</v>
       </c>
@@ -851,12 +851,12 @@
         <v>10</v>
       </c>
       <c r="D3" s="12">
-        <f t="shared" ref="D3:E9" ca="1" si="0">TODAY()-6</f>
-        <v>45263</v>
+        <f t="shared" ref="D3:E5" ca="1" si="0">TODAY()-6</f>
+        <v>45267</v>
       </c>
       <c r="E3" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45263</v>
+        <v>45267</v>
       </c>
       <c r="F3" s="10" t="str">
         <f>IFERROR(IF(ProjectTracker[[#This Row],[Actual Work (in hours)]]=0,"",IF(ABS((ProjectTracker[[#This Row],[Actual Work (in hours)]]-#REF!)/#REF!)&gt;FlagPercent,1,0)),"")</f>
@@ -885,11 +885,11 @@
       </c>
       <c r="D4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45263</v>
+        <v>45267</v>
       </c>
       <c r="E4" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45263</v>
+        <v>45267</v>
       </c>
       <c r="F4" s="10" t="str">
         <f>IFERROR(IF(ProjectTracker[[#This Row],[Actual Work (in hours)]]=0,"",IF(ABS((ProjectTracker[[#This Row],[Actual Work (in hours)]]-#REF!)/#REF!)&gt;FlagPercent,1,0)),"")</f>
@@ -918,11 +918,11 @@
       </c>
       <c r="D5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45263</v>
+        <v>45267</v>
       </c>
       <c r="E5" s="12">
         <f t="shared" ca="1" si="0"/>
-        <v>45263</v>
+        <v>45267</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="8">
@@ -947,7 +947,7 @@
       <c r="I6" s="7"/>
       <c r="J6" s="17"/>
     </row>
-    <row r="7" spans="2:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" ht="55.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
@@ -956,11 +956,11 @@
       </c>
       <c r="D7" s="12">
         <f ca="1">TODAY()-5</f>
-        <v>45264</v>
+        <v>45268</v>
       </c>
       <c r="E7" s="12">
         <f ca="1">TODAY()-4</f>
-        <v>45265</v>
+        <v>45269</v>
       </c>
       <c r="F7" s="10" t="str">
         <f>IFERROR(IF(ProjectTracker[[#This Row],[Actual Work (in hours)]]=0,"",IF(ABS((ProjectTracker[[#This Row],[Actual Work (in hours)]]-#REF!)/#REF!)&gt;FlagPercent,1,0)),"")</f>
@@ -989,11 +989,11 @@
       </c>
       <c r="D8" s="12">
         <f ca="1">TODAY()-5</f>
-        <v>45264</v>
+        <v>45268</v>
       </c>
       <c r="E8" s="12">
         <f ca="1">TODAY()-5</f>
-        <v>45264</v>
+        <v>45268</v>
       </c>
       <c r="F8" s="10" t="str">
         <f>IFERROR(IF(ProjectTracker[[#This Row],[Actual Work (in hours)]]=0,"",IF(ABS((ProjectTracker[[#This Row],[Actual Work (in hours)]]-#REF!)/#REF!)&gt;FlagPercent,1,0)),"")</f>
@@ -1022,11 +1022,11 @@
       </c>
       <c r="D9" s="12">
         <f ca="1">TODAY()-4</f>
-        <v>45265</v>
+        <v>45269</v>
       </c>
       <c r="E9" s="12">
         <f ca="1">TODAY()-4</f>
-        <v>45265</v>
+        <v>45269</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="8">
@@ -1049,11 +1049,11 @@
       </c>
       <c r="D10" s="12">
         <f ca="1">TODAY()</f>
-        <v>45269</v>
+        <v>45273</v>
       </c>
       <c r="E10" s="12">
         <f ca="1">TODAY()</f>
-        <v>45269</v>
+        <v>45273</v>
       </c>
       <c r="F10" s="10" t="str">
         <f>IFERROR(IF(ProjectTracker[[#This Row],[Actual Work (in hours)]]=0,"",IF(ABS((ProjectTracker[[#This Row],[Actual Work (in hours)]]-#REF!)/#REF!)&gt;FlagPercent,1,0)),"")</f>
@@ -1073,19 +1073,29 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="2:10" ht="55.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" ht="56" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="D11" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45273</v>
+      </c>
+      <c r="E11" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45273</v>
+      </c>
       <c r="F11" s="10"/>
-      <c r="G11" s="8"/>
+      <c r="G11" s="8">
+        <v>3</v>
+      </c>
       <c r="H11" s="10"/>
-      <c r="I11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="J11" s="17"/>
     </row>
     <row r="12" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1095,12 +1105,22 @@
       <c r="C12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
+      <c r="D12" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45273</v>
+      </c>
+      <c r="E12" s="12">
+        <f ca="1">TODAY()</f>
+        <v>45273</v>
+      </c>
       <c r="F12" s="10"/>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8">
+        <v>3</v>
+      </c>
       <c r="H12" s="10"/>
-      <c r="I12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="J12" s="17"/>
     </row>
     <row r="13" spans="2:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>